<commit_message>
nuevos requisitos para el viernes 14
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="82">
   <si>
     <t>REQUISITOS</t>
   </si>
@@ -261,6 +261,18 @@
   </si>
   <si>
     <t>Prototipo de Interfaz web</t>
+  </si>
+  <si>
+    <t>caca</t>
+  </si>
+  <si>
+    <t>viernes 14</t>
+  </si>
+  <si>
+    <t>Prototipo de motor de reglas para el horario</t>
+  </si>
+  <si>
+    <t>al generar un horario  cumple con los demas requisitos</t>
   </si>
 </sst>
 </file>
@@ -642,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -1247,7 +1259,27 @@
         <v>20</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="21" x14ac:dyDescent="0.15">
+      <c r="B31" s="1">
+        <v>30</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G31" s="1">
+        <v>100</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ultimo requisito con grupos de profes añadido
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="112">
   <si>
     <t>REQUISITOS</t>
   </si>
@@ -357,6 +357,12 @@
   </si>
   <si>
     <t>Las sesiones no pueden estar separadas por mas de X horas de clases configurables.</t>
+  </si>
+  <si>
+    <t>Crear grupos de profesores</t>
+  </si>
+  <si>
+    <t>Todas las restricciones que tenga un profesor se le pueden aplicar a determinado grupo de profesores aunque con un menor peso que las restricciones aplicadas a cada profesor individual (las restricciones individuales sobreescriben a las restricciones de grupo) se comprueba aplicando solo una restriccion a un profesor, una como grupo y esta misma como profesor individual para distintas horas, debe coger siempre la restriccion individual por encima de la del grupo.</t>
   </si>
 </sst>
 </file>
@@ -738,10 +744,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:J46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -1520,6 +1526,17 @@
         <v>109</v>
       </c>
     </row>
+    <row r="46" spans="2:4" ht="105" x14ac:dyDescent="0.15">
+      <c r="B46" s="1">
+        <v>45</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>111</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
maximo y minimo numero de horas por dia (profesor)
</commit_message>
<xml_diff>
--- a/Requisitos.xlsx
+++ b/Requisitos.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Repositorio\TimeTableManager\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="24495" windowHeight="14775"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="20730" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -368,7 +363,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -384,7 +379,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -403,6 +398,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -416,7 +423,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -428,6 +435,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -490,7 +503,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -542,7 +555,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -736,7 +749,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -746,14 +759,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="2" width="11" style="1"/>
-    <col min="3" max="4" width="30.625" style="2" customWidth="1"/>
+    <col min="3" max="4" width="30.5703125" style="2" customWidth="1"/>
     <col min="5" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
@@ -1376,25 +1389,25 @@
       <c r="B32" s="1">
         <v>31</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="7" t="s">
         <v>82</v>
       </c>
       <c r="D32" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="33" spans="2:4" ht="31.5" x14ac:dyDescent="0.15">
+    <row r="33" spans="2:4" ht="42" x14ac:dyDescent="0.15">
       <c r="B33" s="1">
         <v>32</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="7" t="s">
         <v>84</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="42" x14ac:dyDescent="0.15">
+    <row r="34" spans="2:4" ht="52.5" x14ac:dyDescent="0.15">
       <c r="B34" s="1">
         <v>33</v>
       </c>
@@ -1405,22 +1418,22 @@
         <v>90</v>
       </c>
     </row>
-    <row r="35" spans="2:4" ht="42" x14ac:dyDescent="0.15">
+    <row r="35" spans="2:4" ht="52.5" x14ac:dyDescent="0.15">
       <c r="B35" s="1">
         <v>34</v>
       </c>
-      <c r="C35" s="2" t="s">
+      <c r="C35" s="7" t="s">
         <v>87</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="52.5" x14ac:dyDescent="0.15">
+    <row r="36" spans="2:4" ht="63" x14ac:dyDescent="0.15">
       <c r="B36" s="1">
         <v>35</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C36" s="8" t="s">
         <v>88</v>
       </c>
       <c r="D36" s="2" t="s">
@@ -1438,7 +1451,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="38" spans="2:4" ht="31.5" x14ac:dyDescent="0.15">
+    <row r="38" spans="2:4" ht="42" x14ac:dyDescent="0.15">
       <c r="B38" s="1">
         <v>37</v>
       </c>
@@ -1449,7 +1462,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="31.5" x14ac:dyDescent="0.15">
+    <row r="39" spans="2:4" ht="42" x14ac:dyDescent="0.15">
       <c r="B39" s="1">
         <v>38</v>
       </c>
@@ -1482,7 +1495,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="42" spans="2:4" ht="84" x14ac:dyDescent="0.15">
+    <row r="42" spans="2:4" ht="105" x14ac:dyDescent="0.15">
       <c r="B42" s="1">
         <v>41</v>
       </c>
@@ -1493,7 +1506,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="2:4" ht="73.5" x14ac:dyDescent="0.15">
+    <row r="43" spans="2:4" ht="84" x14ac:dyDescent="0.15">
       <c r="B43" s="1">
         <v>42</v>
       </c>
@@ -1515,7 +1528,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="45" spans="2:4" ht="21" x14ac:dyDescent="0.15">
+    <row r="45" spans="2:4" ht="31.5" x14ac:dyDescent="0.15">
       <c r="B45" s="1">
         <v>44</v>
       </c>

</xml_diff>